<commit_message>
Updated Format for XLXS
</commit_message>
<xml_diff>
--- a/public/formats/patient-xlxs-import.xlsx
+++ b/public/formats/patient-xlxs-import.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>First Name</t>
   </si>
@@ -46,7 +46,13 @@
     <t>Zip</t>
   </si>
   <si>
-    <t>Phone Number</t>
+    <t>Cellphone</t>
+  </si>
+  <si>
+    <t>Workphone</t>
+  </si>
+  <si>
+    <t>Homephone</t>
   </si>
   <si>
     <t>Gender</t>
@@ -64,7 +70,31 @@
     <t>Severity</t>
   </si>
   <si>
-    <t>Insurance Type</t>
+    <t>Insurance Carrier</t>
+  </si>
+  <si>
+    <t>Subscriber Name</t>
+  </si>
+  <si>
+    <t>Subscriber Dob</t>
+  </si>
+  <si>
+    <t>Subscriber Id</t>
+  </si>
+  <si>
+    <t>Group No</t>
+  </si>
+  <si>
+    <t>Relation To Patient</t>
+  </si>
+  <si>
+    <t>Special Request</t>
+  </si>
+  <si>
+    <t>Preferred Method Of Contact</t>
+  </si>
+  <si>
+    <t>Primary Care Physician</t>
   </si>
   <si>
     <t>Priority</t>
@@ -73,13 +103,13 @@
     <t>Language</t>
   </si>
   <si>
-    <t>John</t>
+    <t>Jen</t>
   </si>
   <si>
     <t>Henry</t>
   </si>
   <si>
-    <t>Doe</t>
+    <t>Test</t>
   </si>
   <si>
     <r>
@@ -95,14 +125,51 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>999-999-9999</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Glaucoma</t>
+  </si>
+  <si>
+    <t>Mild</t>
+  </si>
+  <si>
+    <t>Blue Cross</t>
+  </si>
+  <si>
+    <t>George Washington</t>
+  </si>
+  <si>
+    <t>123nkasd</t>
+  </si>
+  <si>
+    <t>Daughter</t>
+  </si>
+  <si>
+    <t>AC1 Tests</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>Dr. Philip</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="60" formatCode="d/m/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -174,7 +241,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -190,13 +257,16 @@
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1449,7 +1519,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1463,19 +1533,29 @@
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.60156" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.67969" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33594" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.375" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="6.125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" style="1" customWidth="1"/>
     <col min="19" max="19" width="7.875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="7.875" style="1" customWidth="1"/>
-    <col min="21" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="13.125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="18.625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19.125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="7.875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="7.875" style="1" customWidth="1"/>
+    <col min="31" max="256" width="6.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.9" customHeight="1">
@@ -1539,44 +1619,118 @@
       <c r="T1" t="s" s="2">
         <v>19</v>
       </c>
+      <c r="U1" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s" s="2">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" ht="16.9" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E2" s="3">
         <v>36636</v>
       </c>
       <c r="F2" s="2">
-        <v>9876</v>
+        <v>2341</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="L2" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="N2" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s" s="2">
+        <v>36</v>
+      </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="7"/>
+      <c r="R2" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="T2" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="U2" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="V2" s="6">
+        <v>33118</v>
+      </c>
+      <c r="W2" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="X2" s="5">
+        <v>1234</v>
+      </c>
+      <c r="Y2" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="Z2" t="s" s="4">
+        <v>43</v>
+      </c>
+      <c r="AA2" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="AB2" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="s" s="7">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" ht="16.9" customHeight="1">
       <c r="A3" s="5"/>
@@ -1598,7 +1752,17 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
-      <c r="T3" s="7"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="8"/>
     </row>
     <row r="4" ht="16.9" customHeight="1">
       <c r="A4" s="5"/>
@@ -1620,7 +1784,17 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
-      <c r="T4" s="7"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="8"/>
     </row>
     <row r="5" ht="16.9" customHeight="1">
       <c r="A5" s="5"/>
@@ -1642,7 +1816,17 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
-      <c r="T5" s="7"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="8"/>
     </row>
     <row r="6" ht="16.9" customHeight="1">
       <c r="A6" s="5"/>
@@ -1664,7 +1848,17 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
-      <c r="T6" s="7"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="8"/>
     </row>
     <row r="7" ht="16.9" customHeight="1">
       <c r="A7" s="5"/>
@@ -1686,7 +1880,17 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
-      <c r="T7" s="7"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="8"/>
     </row>
     <row r="8" ht="16.9" customHeight="1">
       <c r="A8" s="5"/>
@@ -1708,7 +1912,17 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
-      <c r="T8" s="7"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="8"/>
     </row>
     <row r="9" ht="16.9" customHeight="1">
       <c r="A9" s="5"/>
@@ -1730,7 +1944,17 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
-      <c r="T9" s="7"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="8"/>
     </row>
     <row r="10" ht="16.9" customHeight="1">
       <c r="A10" s="5"/>
@@ -1752,7 +1976,17 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
-      <c r="T10" s="7"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Timezone in Bulk Import - #841 (#1031)
</commit_message>
<xml_diff>
--- a/public/formats/patient-xlxs-import.xlsx
+++ b/public/formats/patient-xlxs-import.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>First Name</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Language</t>
+  </si>
+  <si>
+    <t>Timezone</t>
   </si>
   <si>
     <t>Jen</t>
@@ -161,15 +164,17 @@
   <si>
     <t>English</t>
   </si>
+  <si>
+    <t>EST</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="60" formatCode="d/m/yy"/>
+    <numFmt numFmtId="59" formatCode="d/m/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -241,7 +246,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -251,16 +256,13 @@
     <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1519,7 +1521,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1555,7 +1557,8 @@
     <col min="28" max="28" width="19.125" style="1" customWidth="1"/>
     <col min="29" max="29" width="7.875" style="1" customWidth="1"/>
     <col min="30" max="30" width="7.875" style="1" customWidth="1"/>
-    <col min="31" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="7.875" style="1" customWidth="1"/>
+    <col min="32" max="256" width="6.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.9" customHeight="1">
@@ -1649,87 +1652,93 @@
       <c r="AD1" t="s" s="2">
         <v>29</v>
       </c>
+      <c r="AE1" t="s" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" ht="16.9" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3">
-        <v>36636</v>
+        <v>33118</v>
       </c>
       <c r="F2" s="2">
         <v>2341</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" t="s" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N2" t="s" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O2" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" t="s" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" t="s" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T2" t="s" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U2" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="V2" s="6">
+        <v>41</v>
+      </c>
+      <c r="V2" s="3">
         <v>33118</v>
       </c>
       <c r="W2" t="s" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X2" s="5">
         <v>1234</v>
       </c>
       <c r="Y2" t="s" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z2" t="s" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA2" t="s" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB2" t="s" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AC2" s="5">
         <v>1</v>
       </c>
-      <c r="AD2" t="s" s="7">
-        <v>46</v>
+      <c r="AD2" t="s" s="6">
+        <v>47</v>
+      </c>
+      <c r="AE2" t="s" s="6">
+        <v>48</v>
       </c>
     </row>
     <row r="3" ht="16.9" customHeight="1">
@@ -1762,7 +1771,8 @@
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
-      <c r="AD3" s="8"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
     </row>
     <row r="4" ht="16.9" customHeight="1">
       <c r="A4" s="5"/>
@@ -1794,7 +1804,8 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
-      <c r="AD4" s="8"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
     </row>
     <row r="5" ht="16.9" customHeight="1">
       <c r="A5" s="5"/>
@@ -1826,7 +1837,8 @@
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
-      <c r="AD5" s="8"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
     </row>
     <row r="6" ht="16.9" customHeight="1">
       <c r="A6" s="5"/>
@@ -1858,7 +1870,8 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
-      <c r="AD6" s="8"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
     </row>
     <row r="7" ht="16.9" customHeight="1">
       <c r="A7" s="5"/>
@@ -1890,7 +1903,8 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
-      <c r="AD7" s="8"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
     </row>
     <row r="8" ht="16.9" customHeight="1">
       <c r="A8" s="5"/>
@@ -1922,7 +1936,8 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
-      <c r="AD8" s="8"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
     </row>
     <row r="9" ht="16.9" customHeight="1">
       <c r="A9" s="5"/>
@@ -1954,7 +1969,8 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
-      <c r="AD9" s="8"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
     </row>
     <row r="10" ht="16.9" customHeight="1">
       <c r="A10" s="5"/>
@@ -1986,7 +2002,8 @@
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
-      <c r="AD10" s="8"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
#841 timezone import (#1034)
* Timezone in Bulk Import - #841

* Date Format of MM/DD/YY
</commit_message>
<xml_diff>
--- a/public/formats/patient-xlxs-import.xlsx
+++ b/public/formats/patient-xlxs-import.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>First Name</t>
   </si>
@@ -126,6 +126,9 @@
     </r>
   </si>
   <si>
+    <t>12/31/99</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -172,9 +175,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="d/m/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -246,7 +248,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -254,22 +256,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -293,6 +292,54 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1475407</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>105410</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Shape 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4610100" y="3086100"/>
+          <a:ext cx="370508" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1669,341 +1716,341 @@
       <c r="D2" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="E2" s="3">
-        <v>33118</v>
+      <c r="E2" t="s" s="3">
+        <v>35</v>
       </c>
       <c r="F2" s="2">
         <v>2341</v>
       </c>
       <c r="G2" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>36</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="S2" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="T2" t="s" s="3">
+        <v>41</v>
+      </c>
+      <c r="U2" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="H2" t="s" s="4">
-        <v>35</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" t="s" s="4">
-        <v>38</v>
-      </c>
-      <c r="S2" t="s" s="4">
-        <v>39</v>
-      </c>
-      <c r="T2" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="U2" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="V2" s="3">
-        <v>33118</v>
-      </c>
-      <c r="W2" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="X2" s="5">
+      <c r="W2" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="X2" s="4">
         <v>1234</v>
       </c>
-      <c r="Y2" t="s" s="4">
-        <v>43</v>
-      </c>
-      <c r="Z2" t="s" s="4">
+      <c r="Y2" t="s" s="3">
         <v>44</v>
       </c>
-      <c r="AA2" t="s" s="4">
+      <c r="Z2" t="s" s="3">
         <v>45</v>
       </c>
-      <c r="AB2" t="s" s="4">
+      <c r="AA2" t="s" s="3">
         <v>46</v>
       </c>
-      <c r="AC2" s="5">
+      <c r="AB2" t="s" s="3">
+        <v>47</v>
+      </c>
+      <c r="AC2" s="4">
         <v>1</v>
       </c>
-      <c r="AD2" t="s" s="6">
-        <v>47</v>
-      </c>
-      <c r="AE2" t="s" s="6">
+      <c r="AD2" t="s" s="5">
         <v>48</v>
+      </c>
+      <c r="AE2" t="s" s="5">
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="16.9" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
     </row>
     <row r="4" ht="16.9" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
     </row>
     <row r="5" ht="16.9" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
     </row>
     <row r="6" ht="16.9" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
     </row>
     <row r="7" ht="16.9" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="7"/>
-      <c r="AE7" s="7"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
     </row>
     <row r="8" ht="16.9" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
     </row>
     <row r="9" ht="16.9" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="7"/>
-      <c r="AE9" s="7"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
     </row>
     <row r="10" ht="16.9" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="7"/>
-      <c r="AE10" s="7"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2014,5 +2061,7 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#902 practice level users add practice level patients (#1077)
* #902 practice level users add practice level patients

* #902 new excell file
</commit_message>
<xml_diff>
--- a/public/formats/patient-xlxs-import.xlsx
+++ b/public/formats/patient-xlxs-import.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Patients" sheetId="1" r:id="rId4"/>
+    <sheet name="Patients" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>First Name</t>
   </si>
@@ -117,7 +120,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -126,9 +129,6 @@
     </r>
   </si>
   <si>
-    <t>12/31/99</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -175,10 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -186,16 +183,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
@@ -205,7 +192,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
@@ -244,31 +231,34 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -278,24 +268,77 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -309,7 +352,7 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>105410</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Shape 2"/>
         <xdr:cNvSpPr/>
@@ -334,6 +377,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr lvl="0"/>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -343,7 +387,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -535,7 +579,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -544,7 +588,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -553,7 +597,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -562,7 +606,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -571,7 +615,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -580,7 +624,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -692,8 +736,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -701,14 +745,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -727,7 +771,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -735,7 +779,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -763,7 +807,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -789,7 +833,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -815,7 +859,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -841,7 +885,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -867,7 +911,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -893,7 +937,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -919,7 +963,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -945,7 +989,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -971,7 +1015,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -984,9 +1028,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1002,7 +1052,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1021,7 +1071,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1047,7 +1097,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1073,7 +1123,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1099,7 +1149,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1125,7 +1175,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1151,7 +1201,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1177,7 +1227,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1203,7 +1253,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1229,7 +1279,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1255,7 +1305,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1268,9 +1318,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1283,7 +1339,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1302,7 +1358,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1332,7 +1388,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1358,7 +1414,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1384,7 +1440,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1410,7 +1466,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1436,7 +1492,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1462,7 +1518,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1488,7 +1544,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1514,7 +1570,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1540,7 +1596,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1553,242 +1609,239 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="14.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="11.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.8984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.8984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.59765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.69921875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.3984375" style="1" customWidth="1"/>
+    <col min="12" max="14" width="11.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.09765625" style="1" customWidth="1"/>
     <col min="16" max="16" width="10.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.09765625" style="1" customWidth="1"/>
     <col min="18" max="18" width="11.5" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="13.125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="13.125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="13.125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19.125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="7.875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="7.875" style="1" customWidth="1"/>
-    <col min="31" max="31" width="7.875" style="1" customWidth="1"/>
-    <col min="32" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.8984375" style="1" customWidth="1"/>
+    <col min="20" max="26" width="13.09765625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="18.59765625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19.09765625" style="1" customWidth="1"/>
+    <col min="29" max="31" width="7.8984375" style="1" customWidth="1"/>
+    <col min="32" max="256" width="6.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.9" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:31" ht="16.899999999999999" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="2">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="2">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s" s="2">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s" s="2">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s" s="2">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="2">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s" s="2">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s" s="2">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s" s="2">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s" s="2">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s" s="2">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s" s="2">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s" s="2">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s" s="2">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s" s="2">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" ht="16.9" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:31" ht="16.899999999999999" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s" s="3">
-        <v>35</v>
+      <c r="E2" s="7">
+        <v>36525</v>
       </c>
       <c r="F2" s="2">
         <v>2341</v>
       </c>
-      <c r="G2" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s" s="3">
-        <v>36</v>
+      <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" t="s" s="3">
+      <c r="L2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="M2" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="N2" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>38</v>
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" t="s" s="3">
+      <c r="R2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="S2" t="s" s="3">
+      <c r="T2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T2" t="s" s="3">
+      <c r="U2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="U2" t="s" s="3">
+      <c r="V2" s="7">
+        <v>36525</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="V2" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="W2" t="s" s="3">
-        <v>43</v>
       </c>
       <c r="X2" s="4">
         <v>1234</v>
       </c>
-      <c r="Y2" t="s" s="3">
+      <c r="Y2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Z2" t="s" s="3">
+      <c r="AA2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" t="s" s="3">
+      <c r="AB2" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="AB2" t="s" s="3">
-        <v>47</v>
       </c>
       <c r="AC2" s="4">
         <v>1</v>
       </c>
-      <c r="AD2" t="s" s="5">
+      <c r="AD2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AE2" t="s" s="5">
-        <v>49</v>
-      </c>
     </row>
-    <row r="3" ht="16.9" customHeight="1">
+    <row r="3" spans="1:31" ht="16.899999999999999" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1821,7 +1874,7 @@
       <c r="AD3" s="6"/>
       <c r="AE3" s="6"/>
     </row>
-    <row r="4" ht="16.9" customHeight="1">
+    <row r="4" spans="1:31" ht="16.899999999999999" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1854,7 +1907,7 @@
       <c r="AD4" s="6"/>
       <c r="AE4" s="6"/>
     </row>
-    <row r="5" ht="16.9" customHeight="1">
+    <row r="5" spans="1:31" ht="16.899999999999999" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1887,7 +1940,7 @@
       <c r="AD5" s="6"/>
       <c r="AE5" s="6"/>
     </row>
-    <row r="6" ht="16.9" customHeight="1">
+    <row r="6" spans="1:31" ht="16.899999999999999" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1920,7 +1973,7 @@
       <c r="AD6" s="6"/>
       <c r="AE6" s="6"/>
     </row>
-    <row r="7" ht="16.9" customHeight="1">
+    <row r="7" spans="1:31" ht="16.899999999999999" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1953,7 +2006,7 @@
       <c r="AD7" s="6"/>
       <c r="AE7" s="6"/>
     </row>
-    <row r="8" ht="16.9" customHeight="1">
+    <row r="8" spans="1:31" ht="16.899999999999999" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1986,7 +2039,7 @@
       <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
     </row>
-    <row r="9" ht="16.9" customHeight="1">
+    <row r="9" spans="1:31" ht="16.899999999999999" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2019,7 +2072,7 @@
       <c r="AD9" s="6"/>
       <c r="AE9" s="6"/>
     </row>
-    <row r="10" ht="16.9" customHeight="1">
+    <row r="10" spans="1:31" ht="16.899999999999999" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2054,14 +2107,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>